<commit_message>
additional 30 GPs from google maps
</commit_message>
<xml_diff>
--- a/raw_data/gp_data.xlsx
+++ b/raw_data/gp_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shahraj/Documents/University Work/WISE/Ludovica RA Work/lead_mailers/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CB097B-5714-7145-82E8-D92C0655EB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFB2FE0-AADC-2C47-815D-42FEEC58775B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{5A51D493-C501-6E41-97B4-8421A67028E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="492">
   <si>
     <t>Abbey Medical Practice</t>
   </si>
@@ -1278,13 +1278,247 @@
   </si>
   <si>
     <t>Woodhouse Medical Practice</t>
+  </si>
+  <si>
+    <t>York Street Health Practice</t>
+  </si>
+  <si>
+    <t>68 York Street, Leeds, West Yorkshire, LS9 8AA</t>
+  </si>
+  <si>
+    <t>https://www.nhs.uk/services/gp-surgery/york-street-health-practice/XB86669</t>
+  </si>
+  <si>
+    <t>Ashwell Medical Centre</t>
+  </si>
+  <si>
+    <t>Ashwell Medical Centre, Ashwell Rd, Manningham, Bradford BD8 9DP</t>
+  </si>
+  <si>
+    <t>http://www.ashwellmedicalcentre.co.uk/</t>
+  </si>
+  <si>
+    <t>Thornbury Medical Centre</t>
+  </si>
+  <si>
+    <t>20 Rushton Ave, Bradford BD3 7HZ</t>
+  </si>
+  <si>
+    <t>https://www.thornburymc.co.uk/</t>
+  </si>
+  <si>
+    <t>Haigh Hall Medical Practice</t>
+  </si>
+  <si>
+    <t>Haigh Hall Rd, Greengates, Bradford BD10 9AZ</t>
+  </si>
+  <si>
+    <t>https://affinitycare.nhs.uk/haigh-hall/</t>
+  </si>
+  <si>
+    <t>Dr Fox the Grange Medical Centre</t>
+  </si>
+  <si>
+    <t>Grange Medical Centre</t>
+  </si>
+  <si>
+    <t>Grange Medical Centre, 999 York Rd, Seacroft, Leeds LS14 6NX</t>
+  </si>
+  <si>
+    <t>Private GP Services Leeds</t>
+  </si>
+  <si>
+    <t>Units 4 &amp; 5, Gateway West, East St, Leeds LS9 8DA</t>
+  </si>
+  <si>
+    <t>https://www.privategpservices.co.uk/locations/leeds</t>
+  </si>
+  <si>
+    <t>Leeds City Medical Practice</t>
+  </si>
+  <si>
+    <t>https://leeds-city-medical.gpsurgery.net/</t>
+  </si>
+  <si>
+    <t>1st Floor, Parkside Health Centre, 311 Dewsbury Rd, Leeds LS11 5LQ</t>
+  </si>
+  <si>
+    <t>Riverside Medical Centre</t>
+  </si>
+  <si>
+    <t>Savile Rd, Castleford WF10 1PH</t>
+  </si>
+  <si>
+    <t>http://www.riversidemedicalcentre.co.uk/</t>
+  </si>
+  <si>
+    <t>The Leeds Private GP</t>
+  </si>
+  <si>
+    <t>Nuffield Health Leeds Hospital, 2 Leighton St, Leeds LS1 3EB</t>
+  </si>
+  <si>
+    <t>http://www.leedsprivategp.co.uk/</t>
+  </si>
+  <si>
+    <t>Manor Medical Practice - Allerton</t>
+  </si>
+  <si>
+    <t>Bell Dean Rd, Allerton, Bradford BD15 7WA</t>
+  </si>
+  <si>
+    <t>https://www.manor-bradford.co.uk/</t>
+  </si>
+  <si>
+    <t>Hillside Bridge Health Centre, 4 Butler St W, Bradford BD3 0BS</t>
+  </si>
+  <si>
+    <t>New Otley Road Medical</t>
+  </si>
+  <si>
+    <t>https://www.drakbarssurgery.nhs.uk/index.aspx?</t>
+  </si>
+  <si>
+    <t>Middleton Park GP Surgery</t>
+  </si>
+  <si>
+    <t>Middleton Park Ave, Middleton, Leeds LS10 4HT</t>
+  </si>
+  <si>
+    <t>http://www.middletonparkgpsurgery.co.uk/</t>
+  </si>
+  <si>
+    <t>Oakwood Lane Medical Practice</t>
+  </si>
+  <si>
+    <t>2 Amberton Terrace, Leeds LS8 3BZ</t>
+  </si>
+  <si>
+    <t>http://www.oakwoodlanemedical.nhs.uk/</t>
+  </si>
+  <si>
+    <t>Springfield Surgery</t>
+  </si>
+  <si>
+    <t>Canalside Health Care Centre, 2 Kingsway, Bingley BD16 4RP</t>
+  </si>
+  <si>
+    <t>http://www.springfieldsurgery.nhs.uk/</t>
+  </si>
+  <si>
+    <t>The Bradford Moor Practice</t>
+  </si>
+  <si>
+    <t>http://www.bradfordmoorpractice.co.uk/</t>
+  </si>
+  <si>
+    <t>Barkerend Health Centre Daffodil Building, Barkerend Rd, Bradford BD3 8QH</t>
+  </si>
+  <si>
+    <t>The Whitehall Clinic</t>
+  </si>
+  <si>
+    <t>Whitehall Clinic</t>
+  </si>
+  <si>
+    <t>5 Wellington Pl, Leeds LS1 4AP</t>
+  </si>
+  <si>
+    <t>https://www.whitehallclinic.com/files/price-list-june-2023.pdf</t>
+  </si>
+  <si>
+    <t>Barkerend Health Centre</t>
+  </si>
+  <si>
+    <t>Bevan at York Street Health Practice</t>
+  </si>
+  <si>
+    <t>http://www.wearebevan.co.uk/</t>
+  </si>
+  <si>
+    <t>The Avenue Clinic Leeds</t>
+  </si>
+  <si>
+    <t>24 The Avenue, Leeds LS17 7BE</t>
+  </si>
+  <si>
+    <t>http://www.theavenueclinic.co.uk/</t>
+  </si>
+  <si>
+    <t>Dekeyser Group Practice</t>
+  </si>
+  <si>
+    <t>http://www.fountainmedical.co.uk/</t>
+  </si>
+  <si>
+    <t>The Fountain Medical Centre, Little Fountain St, Morley, Leeds LS27 9EN</t>
+  </si>
+  <si>
+    <t>Shenstone House Surgery</t>
+  </si>
+  <si>
+    <t>Shenstone House Surgery, Elland Rd, Leeds LS27 7PX</t>
+  </si>
+  <si>
+    <t>http://www.windsorhousegrouppractice.co.uk/</t>
+  </si>
+  <si>
+    <t>Cherry Tree Surgery</t>
+  </si>
+  <si>
+    <t>Batley Health Centre, 132 Upper Commercial St, Batley WF17 5DH</t>
+  </si>
+  <si>
+    <t>https://www.cherrytreesurgery.co.uk/</t>
+  </si>
+  <si>
+    <t>Stanley Health Centre</t>
+  </si>
+  <si>
+    <t>Lake Lock Road Stanley, Lake Lock Rd, Stanley, Wakefield WF3 4HS</t>
+  </si>
+  <si>
+    <t>Morris Lane Surgery</t>
+  </si>
+  <si>
+    <t>15 Morris Ln, Kirkstall, Leeds LS5 3DB</t>
+  </si>
+  <si>
+    <t>Health Care First - Pinfold Surgery</t>
+  </si>
+  <si>
+    <t>Pinfold Ln, Mickletown Methley, Methley, Leeds LS26 9LA</t>
+  </si>
+  <si>
+    <t>Health Care First - Castleford Health Centre</t>
+  </si>
+  <si>
+    <t>Castleford Health Centre, Welbeck St, Castleford WF10 1DP</t>
+  </si>
+  <si>
+    <t>Spire Methley Park Private GP Surgery</t>
+  </si>
+  <si>
+    <t>Spire Methley Park Hospital, Methley Ln, Methley, Leeds LS26 9HG</t>
+  </si>
+  <si>
+    <t>https://www.spirehealthcare.com/spire-methley-park-hospital/treatments/private-gp-services/?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=SpireGP_GMB</t>
+  </si>
+  <si>
+    <t>Spire Leeds Private GP Surgery</t>
+  </si>
+  <si>
+    <t>Spire, Hospital, Jackson Ave, Roundhay, Leeds LS8 1NT</t>
+  </si>
+  <si>
+    <t>https://www.spirehealthcare.com/spire-leeds-hospital/treatments/private-gp-services/?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=SpireGP_GMB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1336,6 +1570,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1358,7 +1607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1369,13 +1618,86 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1408,19 +1730,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9654196A-E9DF-2F4E-AAB0-73D66431205C}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9654196A-E9DF-2F4E-AAB0-73D66431205C}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
   <autoFilter ref="A1:G1048576" xr:uid="{9654196A-E9DF-2F4E-AAB0-73D66431205C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1048576">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G188">
     <sortCondition ref="B1:B1048576"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3BC6A36C-DDFC-B940-8B4C-D55D3BBC8F85}" name="gp_name"/>
-    <tableColumn id="2" xr3:uid="{F0E50E81-4F44-8746-B2E5-723F800BA7E7}" name="unique_name"/>
-    <tableColumn id="3" xr3:uid="{DDFA7F42-F049-4C43-ADAE-35A74E845524}" name="address"/>
-    <tableColumn id="4" xr3:uid="{9F9D9E42-EE36-594F-BF91-EA65C6DD9E14}" name="website"/>
-    <tableColumn id="5" xr3:uid="{4BD6D769-67F1-1149-9933-0A07DAAD0712}" name="notes"/>
-    <tableColumn id="6" xr3:uid="{CFF31EDA-9FD0-8845-981D-B0F36D3BB4DC}" name="exclude"/>
-    <tableColumn id="7" xr3:uid="{B74BFFE3-A54E-8645-A838-6DFE307C5C0E}" name="reason_if_exclude"/>
+    <tableColumn id="1" xr3:uid="{3BC6A36C-DDFC-B940-8B4C-D55D3BBC8F85}" name="gp_name" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F0E50E81-4F44-8746-B2E5-723F800BA7E7}" name="unique_name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{DDFA7F42-F049-4C43-ADAE-35A74E845524}" name="address" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{9F9D9E42-EE36-594F-BF91-EA65C6DD9E14}" name="website" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4BD6D769-67F1-1149-9933-0A07DAAD0712}" name="notes" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{CFF31EDA-9FD0-8845-981D-B0F36D3BB4DC}" name="exclude" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B74BFFE3-A54E-8645-A838-6DFE307C5C0E}" name="reason_if_exclude" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1743,19 +2065,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FD9AE3-9F49-7D4C-96D9-D53606D2621F}">
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="92" workbookViewId="0">
+      <selection activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="59.6640625" customWidth="1"/>
-    <col min="3" max="3" width="60.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" customWidth="1"/>
+    <col min="1" max="2" width="59.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="60.1640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="8"/>
+    <col min="7" max="7" width="17.1640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1934,23 +2257,22 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="E12" s="1"/>
+      <c r="A12" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>367</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>367</v>
@@ -1961,73 +2283,73 @@
       <c r="D13" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>335</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>335</v>
+        <v>367</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>335</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>117</v>
+        <v>335</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>119</v>
+        <v>4</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
@@ -2042,1195 +2364,1178 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>336</v>
+        <v>121</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>348</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>348</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>8</v>
+        <v>348</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>348</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>127</v>
+        <v>349</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>338</v>
+        <v>127</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>344</v>
+        <v>9</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>124</v>
+        <v>13</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>126</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>126</v>
+      <c r="A26" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>16</v>
+        <v>337</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>346</v>
+        <v>137</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>347</v>
+        <v>205</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>142</v>
+        <v>346</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>144</v>
+        <v>347</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>350</v>
+        <v>21</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>350</v>
+        <v>21</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>356</v>
+        <v>22</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>356</v>
+        <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>26</v>
+        <v>350</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E38" s="1"/>
+      <c r="A38" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>376</v>
+        <v>158</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>374</v>
+        <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>174</v>
+        <v>369</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>36</v>
+        <v>373</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>36</v>
+        <v>373</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>376</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>163</v>
+        <v>375</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>164</v>
+        <v>376</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>363</v>
+        <v>35</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>364</v>
+        <v>35</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>364</v>
+        <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>370</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>37</v>
+        <v>364</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>37</v>
+        <v>364</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>38</v>
+        <v>363</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>38</v>
+        <v>364</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>372</v>
+        <v>163</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>380</v>
+        <v>29</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>381</v>
+        <v>163</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E48" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>183</v>
+        <v>371</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>187</v>
+        <v>372</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>189</v>
+      <c r="A51" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E52" s="1"/>
+      <c r="A52" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E53" s="1"/>
+      <c r="A53" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>45</v>
+        <v>380</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>45</v>
+        <v>380</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>194</v>
+        <v>381</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>384</v>
+        <v>41</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>384</v>
+        <v>41</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>132</v>
+      <c r="A57" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E58" s="1"/>
+      <c r="A58" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E59" s="1"/>
+        <v>383</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>358</v>
+        <v>42</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>359</v>
+        <v>42</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>360</v>
+        <v>191</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>159</v>
+        <v>341</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>160</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>49</v>
+        <v>384</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>49</v>
+        <v>384</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>384</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>207</v>
+        <v>385</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>52</v>
+        <v>359</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>52</v>
+        <v>359</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>209</v>
+        <v>159</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>360</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>386</v>
+        <v>358</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>53</v>
+        <v>359</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>211</v>
+        <v>159</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>360</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>53</v>
+        <v>357</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>53</v>
+        <v>359</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>211</v>
+        <v>159</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>360</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>387</v>
+        <v>27</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>54</v>
+        <v>359</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>212</v>
+        <v>159</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="E70" s="1"/>
+        <v>360</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>215</v>
+        <v>201</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>202</v>
       </c>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>216</v>
+        <v>50</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="E74" s="1"/>
+      <c r="A74" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>221</v>
+        <v>206</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>388</v>
+        <v>208</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>60</v>
+        <v>386</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>389</v>
+        <v>53</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>389</v>
+        <v>53</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>228</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>390</v>
+        <v>54</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>391</v>
+        <v>212</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C91" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D91" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C92" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D92" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D93" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D95" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D96" s="6" t="s">
         <v>252</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E85" s="1"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E86" s="1"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="E94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="E95" s="1"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>132</v>
@@ -3238,1104 +3543,1544 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>73</v>
+        <v>394</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>249</v>
+        <v>181</v>
       </c>
       <c r="E97" s="1"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>254</v>
+        <v>181</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>258</v>
+        <v>234</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="E100" s="1"/>
+      <c r="A100" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>79</v>
+        <v>379</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>79</v>
+        <v>379</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>261</v>
+        <v>184</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>262</v>
+        <v>185</v>
       </c>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>108</v>
+        <v>378</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E103" s="1"/>
-      <c r="F103"/>
-      <c r="G103"/>
+        <v>379</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F103" s="8"/>
+      <c r="G103" s="8"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>264</v>
+        <v>238</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1" t="s">
-        <v>266</v>
+      <c r="A105" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>268</v>
+        <v>395</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>138</v>
+        <v>244</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>139</v>
+        <v>246</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>400</v>
+        <v>72</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>210</v>
+        <v>247</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>401</v>
+        <v>72</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E110" s="1"/>
+        <v>247</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E114" s="1"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E123" s="1"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E124" s="1"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C127" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="B128" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E111" s="1"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
+      <c r="E128" s="1"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B129" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C129" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D112" s="8" t="s">
+      <c r="D129" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B130" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D113" s="8" t="s">
+      <c r="D130" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="E130" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E114" s="1"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
+      <c r="E131" s="1"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C132" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D132" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E132" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="2" t="s">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="D133" s="8" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="D135" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B136" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D116" s="6" t="s">
+      <c r="D136" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="E116" s="1"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="2" t="s">
+      <c r="E136" s="1"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B138" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D138" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E117" s="1"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" s="2" t="s">
+      <c r="E138" s="1"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B139" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C139" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D118" s="6" t="s">
+      <c r="D139" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="2" t="s">
+      <c r="E139" s="1"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D119" s="6" t="s">
+      <c r="D140" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="E119" s="1"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" s="2" t="s">
+      <c r="E140" s="1"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="D141" s="8" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="D143" s="8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C144" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D144" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E120" s="1"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E121" s="1"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E122" s="1"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E123" s="1"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A124" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D124" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E124" s="1"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D125" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A126" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="E126" s="1"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="E128" s="1"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E130" s="1"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E131" s="1"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="E132" s="1"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D133" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="E133" s="1"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E134" s="1"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E135" s="1"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E136" s="1"/>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E137" s="1"/>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E138" s="1"/>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D139" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E139" s="1"/>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E140" s="1"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D141" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D142" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C143" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D143" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E143" s="1"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C144" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D144" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="E144" s="1"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B145" s="2"/>
-      <c r="C145" s="1"/>
-      <c r="D145" s="1"/>
-      <c r="E145" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F145" t="s">
-        <v>327</v>
-      </c>
-      <c r="G145" t="s">
-        <v>328</v>
-      </c>
+        <v>342</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E145" s="1"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B146" s="2"/>
-      <c r="C146" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>353</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E146" s="1"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B147" s="2"/>
-      <c r="C147" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="D147" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>354</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="E147" s="1"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B148" s="2"/>
-      <c r="C148" s="7" t="s">
-        <v>162</v>
+        <v>365</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="F148" t="s">
-        <v>327</v>
-      </c>
-      <c r="G148" t="s">
-        <v>361</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="E148" s="1"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B149" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="C149" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F149" t="s">
-        <v>327</v>
-      </c>
-      <c r="G149" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B150" s="2"/>
+        <v>351</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>351</v>
+      </c>
       <c r="C150" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D150" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F150" t="s">
-        <v>327</v>
-      </c>
-      <c r="G150" t="s">
-        <v>353</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
-      <c r="F151" t="s">
+        <v>23</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F151" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="G151" t="s">
-        <v>353</v>
+      <c r="G151" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="1"/>
-      <c r="D152" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F152" t="s">
-        <v>327</v>
-      </c>
-      <c r="G152" t="s">
-        <v>361</v>
+      <c r="A152" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="D152" s="8" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B153" s="2"/>
+        <v>396</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>396</v>
+      </c>
       <c r="C153" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>399</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E153" s="1"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B154" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>396</v>
+      </c>
       <c r="C154" s="1" t="s">
-        <v>282</v>
+        <v>241</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>283</v>
+        <v>242</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F154" t="s">
-        <v>327</v>
-      </c>
-      <c r="G154" t="s">
-        <v>361</v>
+        <v>132</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A155" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B155" s="2"/>
-      <c r="C155" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>328</v>
+      <c r="A155" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="D155" s="8" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B156" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C156" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="D156" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>361</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B157" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C157" s="1" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G157" s="1" t="s">
-        <v>361</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="E157" s="1"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="E158" s="1"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="E159" s="1"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E160" s="1"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E161" s="1"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E162" s="1"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="D163" s="8" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="D164" s="8" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E165" s="1"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E166" s="1"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E167" s="1"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E168" s="1"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D169" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D170" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D171" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E171" s="1"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D172" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="D173" s="8" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="D174" s="8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B175" s="2"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F175" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G175" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B176" s="2"/>
+      <c r="C176" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B177" s="2"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B178" s="2"/>
+      <c r="C178" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D178" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F178" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G178" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B179" s="2"/>
+      <c r="C179" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D179" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F179" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G179" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B180" s="2"/>
+      <c r="C180" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D180" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F180" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G180" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B181" s="2"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G181" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B182" s="2"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F182" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G182" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B183" s="2"/>
+      <c r="C183" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D183" s="1"/>
+      <c r="E183" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B184" s="2"/>
+      <c r="C184" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D184" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F184" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G184" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B185" s="2"/>
+      <c r="C185" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B186" s="2"/>
+      <c r="C186" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D186" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B187" s="2"/>
+      <c r="C187" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B158" s="2"/>
-      <c r="C158" s="1" t="s">
+      <c r="B188" s="2"/>
+      <c r="C188" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="D188" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="E158" s="1" t="s">
+      <c r="E188" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="F188" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="G158" s="1" t="s">
+      <c r="G188" s="1" t="s">
         <v>361</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D148" r:id="rId1" xr:uid="{8906E0AF-3857-B543-B7A2-FB31843E8864}"/>
-    <hyperlink ref="D45" r:id="rId2" xr:uid="{8ACD1261-13C9-6043-8F54-362A34FF2457}"/>
-    <hyperlink ref="D149" r:id="rId3" xr:uid="{B2C74777-674D-E44B-9F97-EEC06E358E64}"/>
+    <hyperlink ref="D178" r:id="rId1" xr:uid="{8906E0AF-3857-B543-B7A2-FB31843E8864}"/>
+    <hyperlink ref="D48" r:id="rId2" xr:uid="{8ACD1261-13C9-6043-8F54-362A34FF2457}"/>
+    <hyperlink ref="D179" r:id="rId3" xr:uid="{B2C74777-674D-E44B-9F97-EEC06E358E64}"/>
     <hyperlink ref="D11" r:id="rId4" xr:uid="{40EAC001-CE45-9041-A96B-463AA39DD428}"/>
-    <hyperlink ref="D38" r:id="rId5" xr:uid="{B1630857-CF06-3346-B983-D648169AB468}"/>
-    <hyperlink ref="D41" r:id="rId6" xr:uid="{46B12B2E-6394-154E-AEDF-8AA7FF4F2580}"/>
-    <hyperlink ref="D47" r:id="rId7" xr:uid="{65D3F06A-0249-CE44-8B21-232C6761B444}"/>
-    <hyperlink ref="D150" r:id="rId8" xr:uid="{E01A6B35-AD7F-0C41-B75F-C4A3C74BEE85}"/>
-    <hyperlink ref="D144" r:id="rId9" xr:uid="{03889B6A-5A3D-0A47-96F4-5B7F7A343DD8}"/>
-    <hyperlink ref="D49" r:id="rId10" xr:uid="{B0B59049-69A1-054B-935F-1A3792C066AE}"/>
-    <hyperlink ref="D90" r:id="rId11" xr:uid="{AF472C2E-2B02-404E-A5D3-7B7F30AF9816}"/>
-    <hyperlink ref="D51" r:id="rId12" xr:uid="{27E9A21C-AE07-204C-A73E-8A557B111120}"/>
-    <hyperlink ref="D57" r:id="rId13" xr:uid="{F05BD9E5-5182-D04D-8AE5-08529F401B79}"/>
-    <hyperlink ref="D54" r:id="rId14" xr:uid="{2559210C-1153-7546-AEF7-7020CF877C2D}"/>
-    <hyperlink ref="D55" r:id="rId15" xr:uid="{89535B52-83C0-2548-BC7F-78859B314482}"/>
-    <hyperlink ref="D58" r:id="rId16" xr:uid="{67F22A09-F1A5-C54B-BF9C-1BDB262930C4}"/>
-    <hyperlink ref="D63" r:id="rId17" xr:uid="{F790D20E-F119-A64C-AAEB-79AABB72EAC6}"/>
-    <hyperlink ref="D64" r:id="rId18" xr:uid="{9C09EDAF-7B31-4F45-BCFF-C48C392EB062}"/>
-    <hyperlink ref="D67" r:id="rId19" xr:uid="{161C6545-B321-F742-9078-16236A16FB31}"/>
-    <hyperlink ref="D69" r:id="rId20" xr:uid="{B5806F9D-C8C3-7F4A-AD2F-A650D0AD7C23}"/>
-    <hyperlink ref="D71" r:id="rId21" xr:uid="{A46D6932-D76B-5844-B828-4BAD6BEDE8A3}"/>
-    <hyperlink ref="D74" r:id="rId22" xr:uid="{ABCD2EF1-AEE3-2340-968D-C30066A3FDB6}"/>
-    <hyperlink ref="D75" r:id="rId23" xr:uid="{9DB06AB9-6C09-0344-A055-49BD6AE41838}"/>
-    <hyperlink ref="D76" r:id="rId24" xr:uid="{A0998689-882F-A94D-A1C5-544EEF90C41E}"/>
-    <hyperlink ref="D77" r:id="rId25" xr:uid="{B3FD57D4-1358-044C-8FAE-28427DF77FA4}"/>
-    <hyperlink ref="D152" r:id="rId26" xr:uid="{78856CA9-64E1-3E46-B4A6-E438F3A85C64}"/>
-    <hyperlink ref="D78" r:id="rId27" xr:uid="{3D6D5FC5-0516-3648-85B6-FFFA43F4969F}"/>
-    <hyperlink ref="D81" r:id="rId28" xr:uid="{979822BB-0EF1-B843-BCC5-09CA94A7AE86}"/>
-    <hyperlink ref="D82" r:id="rId29" xr:uid="{96933218-6BBA-AE45-8752-1A9B850237D9}"/>
-    <hyperlink ref="D86" r:id="rId30" xr:uid="{44BA42DB-57C8-1B4B-801D-BDE90BB35020}"/>
-    <hyperlink ref="D87" r:id="rId31" xr:uid="{37A0B43E-A425-E040-9320-815C838AFB01}"/>
-    <hyperlink ref="D88" r:id="rId32" xr:uid="{861AA878-B46B-3A49-BD1C-E62DD8AE1FBF}"/>
-    <hyperlink ref="D91" r:id="rId33" xr:uid="{42B80B7A-77E2-C44C-BE4C-A8708DF8758B}"/>
-    <hyperlink ref="D92" r:id="rId34" xr:uid="{B143DC82-4B94-FB4D-949E-16D675A0D1E5}"/>
-    <hyperlink ref="D129" r:id="rId35" xr:uid="{022CA260-472B-544B-BA84-8E7AB6B788FB}"/>
-    <hyperlink ref="D93" r:id="rId36" xr:uid="{73B8D129-8B0B-2443-8FF6-83CA59E6EFF8}"/>
-    <hyperlink ref="D94" r:id="rId37" xr:uid="{38A7A63E-18FC-CF42-BE04-3773BA1E6F54}"/>
-    <hyperlink ref="D97" r:id="rId38" xr:uid="{EBD79BE9-51F8-F040-A177-14A032EC9A62}"/>
-    <hyperlink ref="D84" r:id="rId39" xr:uid="{D22B49EC-5997-454C-A486-D5DD08C6DA71}"/>
-    <hyperlink ref="D98" r:id="rId40" xr:uid="{A9B35213-8B8F-3E41-B594-5476CBA0D57F}"/>
-    <hyperlink ref="D101" r:id="rId41" xr:uid="{E7BB4102-081B-E24F-ADF2-CF0C105922E5}"/>
-    <hyperlink ref="D102" r:id="rId42" xr:uid="{93199EE0-1D61-9E4D-AD91-628FAB2CBF8C}"/>
-    <hyperlink ref="D107" r:id="rId43" xr:uid="{A0E9E395-8154-554B-9D28-16AA5FF935AA}"/>
-    <hyperlink ref="D108" r:id="rId44" xr:uid="{4F631E37-BBF4-8F4C-8633-2C75878DEE35}"/>
-    <hyperlink ref="D109" r:id="rId45" xr:uid="{D8C61CCF-9511-2D4D-859D-162EDE059DA2}"/>
-    <hyperlink ref="D116" r:id="rId46" xr:uid="{E71472A8-6C43-5B40-A852-686FF416BBDB}"/>
-    <hyperlink ref="D118" r:id="rId47" xr:uid="{B7AFE50E-5D4D-2449-A3BB-DB53E5B4B123}"/>
-    <hyperlink ref="D154" r:id="rId48" xr:uid="{4EF7D46E-0CDF-7C46-906A-D6295F9B71EF}"/>
-    <hyperlink ref="D119" r:id="rId49" xr:uid="{EF33740E-62A1-D145-BA6E-065D65211150}"/>
-    <hyperlink ref="D100" r:id="rId50" xr:uid="{2EE985DE-AFD9-7342-849D-48D2B36A1DD5}"/>
-    <hyperlink ref="D133" r:id="rId51" xr:uid="{79C0F84D-CFC7-3F4C-BA0B-8C31140CBB2D}"/>
-    <hyperlink ref="D139" r:id="rId52" xr:uid="{0BE254ED-CFEA-B748-BEA8-BE93F410B53E}"/>
-    <hyperlink ref="D142" r:id="rId53" xr:uid="{DB832EC1-64A5-7748-8F69-8530F991E577}"/>
-    <hyperlink ref="D44" r:id="rId54" xr:uid="{5B5F8F72-8097-0A46-82BF-D6FFEEE40D8F}"/>
-    <hyperlink ref="D43" r:id="rId55" xr:uid="{1BAD97A4-AA1F-684D-A937-7BE83F24453E}"/>
-    <hyperlink ref="D124" r:id="rId56" xr:uid="{1D22C4DA-B79E-9546-BDE2-146CAB934954}"/>
-    <hyperlink ref="D125" r:id="rId57" xr:uid="{4B62CDC6-21D0-7A41-8A4D-EB465F849D55}"/>
+    <hyperlink ref="D41" r:id="rId5" xr:uid="{B1630857-CF06-3346-B983-D648169AB468}"/>
+    <hyperlink ref="D44" r:id="rId6" xr:uid="{46B12B2E-6394-154E-AEDF-8AA7FF4F2580}"/>
+    <hyperlink ref="D50" r:id="rId7" xr:uid="{65D3F06A-0249-CE44-8B21-232C6761B444}"/>
+    <hyperlink ref="D180" r:id="rId8" xr:uid="{E01A6B35-AD7F-0C41-B75F-C4A3C74BEE85}"/>
+    <hyperlink ref="D172" r:id="rId9" xr:uid="{03889B6A-5A3D-0A47-96F4-5B7F7A343DD8}"/>
+    <hyperlink ref="D55" r:id="rId10" xr:uid="{B0B59049-69A1-054B-935F-1A3792C066AE}"/>
+    <hyperlink ref="D103" r:id="rId11" xr:uid="{AF472C2E-2B02-404E-A5D3-7B7F30AF9816}"/>
+    <hyperlink ref="D59" r:id="rId12" xr:uid="{27E9A21C-AE07-204C-A73E-8A557B111120}"/>
+    <hyperlink ref="D65" r:id="rId13" xr:uid="{F05BD9E5-5182-D04D-8AE5-08529F401B79}"/>
+    <hyperlink ref="D62" r:id="rId14" xr:uid="{2559210C-1153-7546-AEF7-7020CF877C2D}"/>
+    <hyperlink ref="D63" r:id="rId15" xr:uid="{89535B52-83C0-2548-BC7F-78859B314482}"/>
+    <hyperlink ref="D66" r:id="rId16" xr:uid="{67F22A09-F1A5-C54B-BF9C-1BDB262930C4}"/>
+    <hyperlink ref="D71" r:id="rId17" xr:uid="{F790D20E-F119-A64C-AAEB-79AABB72EAC6}"/>
+    <hyperlink ref="D72" r:id="rId18" xr:uid="{9C09EDAF-7B31-4F45-BCFF-C48C392EB062}"/>
+    <hyperlink ref="D76" r:id="rId19" xr:uid="{161C6545-B321-F742-9078-16236A16FB31}"/>
+    <hyperlink ref="D78" r:id="rId20" xr:uid="{B5806F9D-C8C3-7F4A-AD2F-A650D0AD7C23}"/>
+    <hyperlink ref="D80" r:id="rId21" xr:uid="{A46D6932-D76B-5844-B828-4BAD6BEDE8A3}"/>
+    <hyperlink ref="D84" r:id="rId22" xr:uid="{ABCD2EF1-AEE3-2340-968D-C30066A3FDB6}"/>
+    <hyperlink ref="D85" r:id="rId23" xr:uid="{9DB06AB9-6C09-0344-A055-49BD6AE41838}"/>
+    <hyperlink ref="D86" r:id="rId24" xr:uid="{A0998689-882F-A94D-A1C5-544EEF90C41E}"/>
+    <hyperlink ref="D88" r:id="rId25" xr:uid="{B3FD57D4-1358-044C-8FAE-28427DF77FA4}"/>
+    <hyperlink ref="D182" r:id="rId26" xr:uid="{78856CA9-64E1-3E46-B4A6-E438F3A85C64}"/>
+    <hyperlink ref="D89" r:id="rId27" xr:uid="{3D6D5FC5-0516-3648-85B6-FFFA43F4969F}"/>
+    <hyperlink ref="D92" r:id="rId28" xr:uid="{979822BB-0EF1-B843-BCC5-09CA94A7AE86}"/>
+    <hyperlink ref="D93" r:id="rId29" xr:uid="{96933218-6BBA-AE45-8752-1A9B850237D9}"/>
+    <hyperlink ref="D98" r:id="rId30" xr:uid="{44BA42DB-57C8-1B4B-801D-BDE90BB35020}"/>
+    <hyperlink ref="D99" r:id="rId31" xr:uid="{37A0B43E-A425-E040-9320-815C838AFB01}"/>
+    <hyperlink ref="D101" r:id="rId32" xr:uid="{861AA878-B46B-3A49-BD1C-E62DD8AE1FBF}"/>
+    <hyperlink ref="D104" r:id="rId33" xr:uid="{42B80B7A-77E2-C44C-BE4C-A8708DF8758B}"/>
+    <hyperlink ref="D106" r:id="rId34" xr:uid="{B143DC82-4B94-FB4D-949E-16D675A0D1E5}"/>
+    <hyperlink ref="D154" r:id="rId35" xr:uid="{022CA260-472B-544B-BA84-8E7AB6B788FB}"/>
+    <hyperlink ref="D107" r:id="rId36" xr:uid="{73B8D129-8B0B-2443-8FF6-83CA59E6EFF8}"/>
+    <hyperlink ref="D108" r:id="rId37" xr:uid="{38A7A63E-18FC-CF42-BE04-3773BA1E6F54}"/>
+    <hyperlink ref="D111" r:id="rId38" xr:uid="{EBD79BE9-51F8-F040-A177-14A032EC9A62}"/>
+    <hyperlink ref="D96" r:id="rId39" xr:uid="{D22B49EC-5997-454C-A486-D5DD08C6DA71}"/>
+    <hyperlink ref="D113" r:id="rId40" xr:uid="{A9B35213-8B8F-3E41-B594-5476CBA0D57F}"/>
+    <hyperlink ref="D117" r:id="rId41" xr:uid="{E7BB4102-081B-E24F-ADF2-CF0C105922E5}"/>
+    <hyperlink ref="D118" r:id="rId42" xr:uid="{93199EE0-1D61-9E4D-AD91-628FAB2CBF8C}"/>
+    <hyperlink ref="D123" r:id="rId43" xr:uid="{A0E9E395-8154-554B-9D28-16AA5FF935AA}"/>
+    <hyperlink ref="D124" r:id="rId44" xr:uid="{4F631E37-BBF4-8F4C-8633-2C75878DEE35}"/>
+    <hyperlink ref="D125" r:id="rId45" xr:uid="{D8C61CCF-9511-2D4D-859D-162EDE059DA2}"/>
+    <hyperlink ref="D136" r:id="rId46" xr:uid="{E71472A8-6C43-5B40-A852-686FF416BBDB}"/>
+    <hyperlink ref="D139" r:id="rId47" xr:uid="{B7AFE50E-5D4D-2449-A3BB-DB53E5B4B123}"/>
+    <hyperlink ref="D184" r:id="rId48" xr:uid="{4EF7D46E-0CDF-7C46-906A-D6295F9B71EF}"/>
+    <hyperlink ref="D140" r:id="rId49" xr:uid="{EF33740E-62A1-D145-BA6E-065D65211150}"/>
+    <hyperlink ref="D115" r:id="rId50" xr:uid="{2EE985DE-AFD9-7342-849D-48D2B36A1DD5}"/>
+    <hyperlink ref="D159" r:id="rId51" xr:uid="{79C0F84D-CFC7-3F4C-BA0B-8C31140CBB2D}"/>
+    <hyperlink ref="D167" r:id="rId52" xr:uid="{0BE254ED-CFEA-B748-BEA8-BE93F410B53E}"/>
+    <hyperlink ref="D170" r:id="rId53" xr:uid="{DB832EC1-64A5-7748-8F69-8530F991E577}"/>
+    <hyperlink ref="D47" r:id="rId54" xr:uid="{5B5F8F72-8097-0A46-82BF-D6FFEEE40D8F}"/>
+    <hyperlink ref="D46" r:id="rId55" xr:uid="{1BAD97A4-AA1F-684D-A937-7BE83F24453E}"/>
+    <hyperlink ref="D148" r:id="rId56" xr:uid="{1D22C4DA-B79E-9546-BDE2-146CAB934954}"/>
+    <hyperlink ref="D149" r:id="rId57" xr:uid="{4B62CDC6-21D0-7A41-8A4D-EB465F849D55}"/>
     <hyperlink ref="D10" r:id="rId58" xr:uid="{2B356DBD-84E4-7A42-8F5D-34F353D299B7}"/>
-    <hyperlink ref="D143" r:id="rId59" xr:uid="{5F8AFBC8-3956-F345-870C-AC7CF23EA7E0}"/>
-    <hyperlink ref="D48" r:id="rId60" xr:uid="{331FAF3B-43CE-A845-B20C-F6E53B45DB36}"/>
-    <hyperlink ref="D89" r:id="rId61" xr:uid="{D9374D24-7B19-9E47-B5A5-9060C63ABB49}"/>
-    <hyperlink ref="D56" r:id="rId62" xr:uid="{5F7F4CC8-91E2-2149-823D-467A52C03B1E}"/>
-    <hyperlink ref="D68" r:id="rId63" xr:uid="{94C6F2CB-F45A-0644-8FBA-22087E2BD654}"/>
-    <hyperlink ref="D70" r:id="rId64" xr:uid="{5DFFCCF1-629A-6043-8F00-B6846DF875B4}"/>
-    <hyperlink ref="D79" r:id="rId65" xr:uid="{BF87B77A-0FF8-2C40-AECB-135819B44C83}"/>
-    <hyperlink ref="D80" r:id="rId66" xr:uid="{EEFF8E62-C7EC-F643-90DF-5A4048198861}"/>
-    <hyperlink ref="D85" r:id="rId67" xr:uid="{9FC10086-9A9D-474E-9872-F96B8EA02215}"/>
-    <hyperlink ref="D128" r:id="rId68" xr:uid="{779571B8-7207-4948-B1EF-9E84F98C3703}"/>
-    <hyperlink ref="D83" r:id="rId69" xr:uid="{3166CB2B-6030-1D40-A73D-2F745115B699}"/>
-    <hyperlink ref="D156" r:id="rId70" xr:uid="{28C88945-0D58-D148-AF99-2DA778DBF36B}"/>
-    <hyperlink ref="D132" r:id="rId71" xr:uid="{273AA9D1-ED1B-444A-AC05-682FD9AC4A63}"/>
-    <hyperlink ref="D141" r:id="rId72" xr:uid="{3263871D-B237-0A4D-86C8-E098F3BE4A3D}"/>
+    <hyperlink ref="D171" r:id="rId59" xr:uid="{5F8AFBC8-3956-F345-870C-AC7CF23EA7E0}"/>
+    <hyperlink ref="D54" r:id="rId60" xr:uid="{331FAF3B-43CE-A845-B20C-F6E53B45DB36}"/>
+    <hyperlink ref="D102" r:id="rId61" xr:uid="{D9374D24-7B19-9E47-B5A5-9060C63ABB49}"/>
+    <hyperlink ref="D64" r:id="rId62" xr:uid="{5F7F4CC8-91E2-2149-823D-467A52C03B1E}"/>
+    <hyperlink ref="D77" r:id="rId63" xr:uid="{94C6F2CB-F45A-0644-8FBA-22087E2BD654}"/>
+    <hyperlink ref="D79" r:id="rId64" xr:uid="{5DFFCCF1-629A-6043-8F00-B6846DF875B4}"/>
+    <hyperlink ref="D90" r:id="rId65" xr:uid="{BF87B77A-0FF8-2C40-AECB-135819B44C83}"/>
+    <hyperlink ref="D91" r:id="rId66" xr:uid="{EEFF8E62-C7EC-F643-90DF-5A4048198861}"/>
+    <hyperlink ref="D97" r:id="rId67" xr:uid="{9FC10086-9A9D-474E-9872-F96B8EA02215}"/>
+    <hyperlink ref="D153" r:id="rId68" xr:uid="{779571B8-7207-4948-B1EF-9E84F98C3703}"/>
+    <hyperlink ref="D95" r:id="rId69" xr:uid="{3166CB2B-6030-1D40-A73D-2F745115B699}"/>
+    <hyperlink ref="D186" r:id="rId70" xr:uid="{28C88945-0D58-D148-AF99-2DA778DBF36B}"/>
+    <hyperlink ref="D158" r:id="rId71" xr:uid="{273AA9D1-ED1B-444A-AC05-682FD9AC4A63}"/>
+    <hyperlink ref="D169" r:id="rId72" xr:uid="{3263871D-B237-0A4D-86C8-E098F3BE4A3D}"/>
+    <hyperlink ref="D51" r:id="rId73" xr:uid="{9F222D05-8913-E44F-9E44-29103739D303}"/>
+    <hyperlink ref="D52" r:id="rId74" xr:uid="{838EE1F7-0771-F04C-A5B2-DD3F6E1224AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId73"/>
+    <tablePart r:id="rId75"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>